<commit_message>
stats update, tiny fixes
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -12,9 +17,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +32,7 @@
     <author>Maks Marcinowski</author>
   </authors>
   <commentList>
-    <comment ref="K2" authorId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0">
+    <comment ref="P2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0">
+    <comment ref="J4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="0">
+    <comment ref="P4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q4" authorId="0">
+    <comment ref="Q4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -906,8 +911,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2386,42 +2391,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -2471,7 +2476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -2524,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1">
+    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -2577,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
@@ -2630,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -2683,7 +2688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
@@ -2736,7 +2741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1">
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -2805,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -2824,7 +2829,7 @@
       <c r="P8" s="23"/>
       <c r="Q8" s="24"/>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -2843,7 +2848,7 @@
       <c r="P9" s="26"/>
       <c r="Q9" s="27"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>28</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>62</v>
@@ -2945,7 +2950,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>63</v>
@@ -2990,7 +2995,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="34"/>
       <c r="C13" s="32" t="s">
@@ -3025,7 +3030,7 @@
       </c>
       <c r="Q13" s="33"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32" t="s">
@@ -3052,7 +3057,7 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="33"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -3077,7 +3082,7 @@
       <c r="P15" s="32"/>
       <c r="Q15" s="33"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -3098,7 +3103,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="33"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -3119,7 +3124,7 @@
       <c r="P17" s="32"/>
       <c r="Q17" s="33"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -3140,7 +3145,7 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="33"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -3161,7 +3166,7 @@
       <c r="P19" s="32"/>
       <c r="Q19" s="37"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -3180,7 +3185,7 @@
       <c r="P20" s="36"/>
       <c r="Q20" s="37"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -3199,7 +3204,7 @@
       <c r="P21" s="36"/>
       <c r="Q21" s="37"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -3217,7 +3222,7 @@
       <c r="P22" s="36"/>
       <c r="Q22" s="37"/>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1">
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -3236,7 +3241,7 @@
       <c r="P23" s="38"/>
       <c r="Q23" s="39"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>33</v>
       </c>
@@ -3289,7 +3294,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>84</v>
@@ -3338,7 +3343,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -3375,7 +3380,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -3408,7 +3413,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -3433,7 +3438,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -3454,7 +3459,7 @@
       <c r="P29" s="32"/>
       <c r="Q29" s="33"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -3473,7 +3478,7 @@
       <c r="P30" s="32"/>
       <c r="Q30" s="33"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -3492,7 +3497,7 @@
       <c r="P31" s="32"/>
       <c r="Q31" s="33"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -3511,7 +3516,7 @@
       <c r="P32" s="32"/>
       <c r="Q32" s="33"/>
     </row>
-    <row r="33" spans="1:17" ht="15" thickBot="1">
+    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -3556,35 +3561,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>138</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -3699,7 +3704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -3758,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>24</v>
       </c>
@@ -3817,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
@@ -3876,7 +3881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
@@ -3935,7 +3940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -4012,7 +4017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4033,7 +4038,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -4054,7 +4059,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>28</v>
       </c>
@@ -4111,7 +4116,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" t="s">
         <v>198</v>
@@ -4162,7 +4167,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>201</v>
@@ -4209,7 +4214,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>200</v>
@@ -4248,7 +4253,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>199</v>
@@ -4281,7 +4286,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>169</v>
@@ -4308,7 +4313,7 @@
       <c r="R15" s="32"/>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>170</v>
@@ -4335,7 +4340,7 @@
       <c r="R16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -4358,7 +4363,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="33"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -4381,7 +4386,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -4402,7 +4407,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="37"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4423,7 +4428,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4444,7 +4449,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4464,7 +4469,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4510,20 +4515,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -4621,7 +4626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>222</v>
       </c>
@@ -4727,7 +4732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -4831,7 +4836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="45"/>
       <c r="B4" t="s">
         <v>5</v>
@@ -4935,7 +4940,7 @@
         <v>4.2666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" t="s">
         <v>21</v>
@@ -5039,10 +5044,10 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AH6" s="42"/>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
         <v>221</v>
       </c>
@@ -5148,7 +5153,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="45"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -5252,7 +5257,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="45"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -5356,7 +5361,7 @@
         <v>4.5333333333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="45"/>
       <c r="B10" t="s">
         <v>21</v>
@@ -5460,10 +5465,10 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AH11" s="42"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
         <v>223</v>
       </c>
@@ -5525,7 +5530,7 @@
         <v>21.875</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="45"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -5585,7 +5590,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="45"/>
       <c r="B14" t="s">
         <v>5</v>
@@ -5645,7 +5650,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="45"/>
       <c r="B15" t="s">
         <v>21</v>
@@ -5804,21 +5809,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5928,7 +5933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>222</v>
       </c>
@@ -6046,7 +6051,7 @@
         <v>22.529411764705884</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6162,7 +6167,7 @@
         <v>2.6764705882352939</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="45"/>
       <c r="B4" t="s">
         <v>5</v>
@@ -6278,7 +6283,7 @@
         <v>5.3235294117647056</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="45"/>
       <c r="B5" t="s">
         <v>21</v>
@@ -6394,10 +6399,10 @@
         <v>3.6470588235294117</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL6" s="41"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="45" t="s">
         <v>221</v>
       </c>
@@ -6515,7 +6520,7 @@
         <v>23.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="45"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6631,7 +6636,7 @@
         <v>2.0882352941176472</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="45"/>
       <c r="B9" t="s">
         <v>5</v>
@@ -6747,7 +6752,7 @@
         <v>4.8529411764705879</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="45"/>
       <c r="B10" t="s">
         <v>21</v>
@@ -6863,10 +6868,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL11" s="41"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
         <v>223</v>
       </c>
@@ -6895,10 +6900,10 @@
         <v>17</v>
       </c>
       <c r="J12" s="1">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1">
         <v>14</v>
-      </c>
-      <c r="K12" s="1">
-        <v>12</v>
       </c>
       <c r="L12" s="1">
         <v>5</v>
@@ -6929,14 +6934,14 @@
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1">
         <f>SUM(C12:AF12)</f>
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="AL12" s="41">
         <f t="shared" si="1"/>
-        <v>17.899999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="45"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7004,7 +7009,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="45"/>
       <c r="B14" t="s">
         <v>5</v>
@@ -7031,10 +7036,10 @@
         <v>7</v>
       </c>
       <c r="J14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K14" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -7065,14 +7070,14 @@
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1">
         <f>SUM(C14:AF14)</f>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AL14" s="41">
         <f t="shared" si="1"/>
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="45"/>
       <c r="B15" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
analysis extended, stats update
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -1509,9 +1509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1532,35 +1529,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="62">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2309,6 +2285,30 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2577,7 +2577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2587,7 +2587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -2662,267 +2662,267 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="47">
-        <v>3</v>
-      </c>
-      <c r="C2" s="48">
-        <v>1</v>
-      </c>
-      <c r="D2" s="47">
-        <v>3</v>
-      </c>
-      <c r="E2" s="48">
-        <v>2</v>
-      </c>
-      <c r="F2" s="47">
-        <v>3</v>
-      </c>
-      <c r="G2" s="48">
-        <v>3</v>
-      </c>
-      <c r="H2" s="47">
-        <v>2</v>
-      </c>
-      <c r="I2" s="48">
-        <v>3</v>
-      </c>
-      <c r="J2" s="47">
-        <v>3</v>
-      </c>
-      <c r="K2" s="48">
+      <c r="B2" s="46">
+        <v>3</v>
+      </c>
+      <c r="C2" s="47">
+        <v>1</v>
+      </c>
+      <c r="D2" s="46">
+        <v>3</v>
+      </c>
+      <c r="E2" s="47">
+        <v>2</v>
+      </c>
+      <c r="F2" s="46">
+        <v>3</v>
+      </c>
+      <c r="G2" s="47">
+        <v>3</v>
+      </c>
+      <c r="H2" s="46">
+        <v>2</v>
+      </c>
+      <c r="I2" s="47">
+        <v>3</v>
+      </c>
+      <c r="J2" s="46">
+        <v>3</v>
+      </c>
+      <c r="K2" s="47">
         <v>0</v>
       </c>
-      <c r="L2" s="47">
+      <c r="L2" s="46">
         <v>0</v>
       </c>
-      <c r="M2" s="48">
-        <v>2</v>
-      </c>
-      <c r="N2" s="47">
-        <v>1</v>
-      </c>
-      <c r="O2" s="48">
-        <v>2</v>
-      </c>
-      <c r="P2" s="47">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="49">
+      <c r="M2" s="47">
+        <v>2</v>
+      </c>
+      <c r="N2" s="46">
+        <v>1</v>
+      </c>
+      <c r="O2" s="47">
+        <v>2</v>
+      </c>
+      <c r="P2" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="50">
         <v>0</v>
       </c>
-      <c r="C3" s="52">
-        <v>1</v>
-      </c>
-      <c r="D3" s="51">
-        <v>1</v>
-      </c>
-      <c r="E3" s="52">
-        <v>2</v>
-      </c>
-      <c r="F3" s="51">
+      <c r="C3" s="51">
+        <v>1</v>
+      </c>
+      <c r="D3" s="50">
+        <v>1</v>
+      </c>
+      <c r="E3" s="51">
+        <v>2</v>
+      </c>
+      <c r="F3" s="50">
         <v>0</v>
       </c>
-      <c r="G3" s="52">
-        <v>1</v>
-      </c>
-      <c r="H3" s="51">
+      <c r="G3" s="51">
+        <v>1</v>
+      </c>
+      <c r="H3" s="50">
         <v>0</v>
       </c>
-      <c r="I3" s="52">
+      <c r="I3" s="51">
         <v>0</v>
       </c>
-      <c r="J3" s="51">
+      <c r="J3" s="50">
         <v>0</v>
       </c>
-      <c r="K3" s="52">
-        <v>1</v>
-      </c>
-      <c r="L3" s="51">
-        <v>3</v>
-      </c>
-      <c r="M3" s="52">
-        <v>2</v>
-      </c>
-      <c r="N3" s="51">
-        <v>1</v>
-      </c>
-      <c r="O3" s="52">
+      <c r="K3" s="51">
+        <v>1</v>
+      </c>
+      <c r="L3" s="50">
+        <v>3</v>
+      </c>
+      <c r="M3" s="51">
+        <v>2</v>
+      </c>
+      <c r="N3" s="50">
+        <v>1</v>
+      </c>
+      <c r="O3" s="51">
         <v>0</v>
       </c>
-      <c r="P3" s="51">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="53">
+      <c r="P3" s="50">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="52">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="55">
-        <v>1</v>
-      </c>
-      <c r="C4" s="56">
+      <c r="B4" s="54">
+        <v>1</v>
+      </c>
+      <c r="C4" s="55">
         <v>0</v>
       </c>
-      <c r="D4" s="55">
-        <v>1</v>
-      </c>
-      <c r="E4" s="56">
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="55">
         <v>0</v>
       </c>
-      <c r="F4" s="55">
+      <c r="F4" s="54">
         <v>0</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="55">
         <v>0</v>
       </c>
-      <c r="H4" s="55">
+      <c r="H4" s="54">
         <v>0</v>
       </c>
-      <c r="I4" s="56">
-        <v>1</v>
-      </c>
-      <c r="J4" s="55">
-        <v>1</v>
-      </c>
-      <c r="K4" s="56">
-        <v>1</v>
-      </c>
-      <c r="L4" s="55">
-        <v>1</v>
-      </c>
-      <c r="M4" s="56">
+      <c r="I4" s="55">
+        <v>1</v>
+      </c>
+      <c r="J4" s="54">
+        <v>1</v>
+      </c>
+      <c r="K4" s="55">
+        <v>1</v>
+      </c>
+      <c r="L4" s="54">
+        <v>1</v>
+      </c>
+      <c r="M4" s="55">
         <v>0</v>
       </c>
-      <c r="N4" s="55">
-        <v>1</v>
-      </c>
-      <c r="O4" s="56">
+      <c r="N4" s="54">
+        <v>1</v>
+      </c>
+      <c r="O4" s="55">
         <v>0</v>
       </c>
-      <c r="P4" s="55">
+      <c r="P4" s="54">
         <v>0</v>
       </c>
-      <c r="Q4" s="57">
+      <c r="Q4" s="56">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>9</v>
       </c>
-      <c r="C5" s="60">
+      <c r="C5" s="59">
         <v>6</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>11</v>
       </c>
-      <c r="E5" s="60">
-        <v>4</v>
-      </c>
-      <c r="F5" s="59">
+      <c r="E5" s="59">
+        <v>4</v>
+      </c>
+      <c r="F5" s="58">
         <v>14</v>
       </c>
-      <c r="G5" s="60">
+      <c r="G5" s="59">
         <v>13</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="58">
         <v>6</v>
       </c>
-      <c r="I5" s="60">
+      <c r="I5" s="59">
         <v>8</v>
       </c>
-      <c r="J5" s="59">
-        <v>5</v>
-      </c>
-      <c r="K5" s="60">
-        <v>2</v>
-      </c>
-      <c r="L5" s="59">
+      <c r="J5" s="58">
+        <v>5</v>
+      </c>
+      <c r="K5" s="59">
+        <v>2</v>
+      </c>
+      <c r="L5" s="58">
         <v>6</v>
       </c>
-      <c r="M5" s="60">
-        <v>4</v>
-      </c>
-      <c r="N5" s="59">
+      <c r="M5" s="59">
+        <v>4</v>
+      </c>
+      <c r="N5" s="58">
         <v>6</v>
       </c>
-      <c r="O5" s="60">
-        <v>5</v>
-      </c>
-      <c r="P5" s="59">
+      <c r="O5" s="59">
+        <v>5</v>
+      </c>
+      <c r="P5" s="58">
         <v>11</v>
       </c>
-      <c r="Q5" s="61">
+      <c r="Q5" s="60">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="63">
-        <v>5</v>
-      </c>
-      <c r="C6" s="64">
-        <v>3</v>
-      </c>
-      <c r="D6" s="63">
-        <v>5</v>
-      </c>
-      <c r="E6" s="64">
-        <v>1</v>
-      </c>
-      <c r="F6" s="63">
-        <v>1</v>
-      </c>
-      <c r="G6" s="64">
-        <v>1</v>
-      </c>
-      <c r="H6" s="63">
-        <v>2</v>
-      </c>
-      <c r="I6" s="64">
-        <v>3</v>
-      </c>
-      <c r="J6" s="63">
-        <v>2</v>
-      </c>
-      <c r="K6" s="64">
-        <v>4</v>
-      </c>
-      <c r="L6" s="63">
+      <c r="B6" s="62">
+        <v>5</v>
+      </c>
+      <c r="C6" s="63">
+        <v>3</v>
+      </c>
+      <c r="D6" s="62">
+        <v>5</v>
+      </c>
+      <c r="E6" s="63">
+        <v>1</v>
+      </c>
+      <c r="F6" s="62">
+        <v>1</v>
+      </c>
+      <c r="G6" s="63">
+        <v>1</v>
+      </c>
+      <c r="H6" s="62">
+        <v>2</v>
+      </c>
+      <c r="I6" s="63">
+        <v>3</v>
+      </c>
+      <c r="J6" s="62">
+        <v>2</v>
+      </c>
+      <c r="K6" s="63">
+        <v>4</v>
+      </c>
+      <c r="L6" s="62">
         <v>8</v>
       </c>
-      <c r="M6" s="64">
-        <v>2</v>
-      </c>
-      <c r="N6" s="63">
+      <c r="M6" s="63">
+        <v>2</v>
+      </c>
+      <c r="N6" s="62">
         <v>7</v>
       </c>
-      <c r="O6" s="64">
-        <v>1</v>
-      </c>
-      <c r="P6" s="63">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="65">
+      <c r="O6" s="63">
+        <v>1</v>
+      </c>
+      <c r="P6" s="62">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="64">
         <v>7</v>
       </c>
     </row>
@@ -3733,10 +3733,10 @@
     <sortCondition descending="1" ref="E10"/>
   </sortState>
   <conditionalFormatting sqref="B7:Q7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -4688,10 +4688,10 @@
     <sortCondition descending="1" ref="B10"/>
   </sortState>
   <conditionalFormatting sqref="B7:S7">
-    <cfRule type="cellIs" dxfId="61" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="3">
@@ -4711,7 +4711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -4820,7 +4820,7 @@
       </c>
     </row>
     <row r="2" spans="1:34">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="65" t="s">
         <v>130</v>
       </c>
       <c r="B2" t="s">
@@ -4926,7 +4926,7 @@
       </c>
     </row>
     <row r="3" spans="1:34">
-      <c r="A3" s="45"/>
+      <c r="A3" s="65"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -5030,7 +5030,7 @@
       </c>
     </row>
     <row r="4" spans="1:34">
-      <c r="A4" s="45"/>
+      <c r="A4" s="65"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -5134,7 +5134,7 @@
       </c>
     </row>
     <row r="5" spans="1:34">
-      <c r="A5" s="45"/>
+      <c r="A5" s="65"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -5241,7 +5241,7 @@
       <c r="AH6" s="42"/>
     </row>
     <row r="7" spans="1:34">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="65" t="s">
         <v>129</v>
       </c>
       <c r="B7" t="s">
@@ -5347,7 +5347,7 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="45"/>
+      <c r="A8" s="65"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -5451,7 +5451,7 @@
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="45"/>
+      <c r="A9" s="65"/>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -5555,7 +5555,7 @@
       </c>
     </row>
     <row r="10" spans="1:34">
-      <c r="A10" s="45"/>
+      <c r="A10" s="65"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -5662,7 +5662,7 @@
       <c r="AH11" s="42"/>
     </row>
     <row r="12" spans="1:34">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="65" t="s">
         <v>131</v>
       </c>
       <c r="B12" t="s">
@@ -5707,7 +5707,9 @@
       <c r="O12" s="1">
         <v>24</v>
       </c>
-      <c r="P12" s="1"/>
+      <c r="P12" s="1">
+        <v>16</v>
+      </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -5726,15 +5728,15 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1">
         <f>SUM(C12:AF12)</f>
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="AH12" s="41">
         <f>AG12/COUNT(C12:AF12)</f>
-        <v>21.76923076923077</v>
+        <v>21.357142857142858</v>
       </c>
     </row>
     <row r="13" spans="1:34">
-      <c r="A13" s="45"/>
+      <c r="A13" s="65"/>
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -5777,7 +5779,9 @@
       <c r="O13" s="1">
         <v>1</v>
       </c>
-      <c r="P13" s="1"/>
+      <c r="P13" s="1">
+        <v>2</v>
+      </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -5796,15 +5800,15 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1">
         <f>SUM(C13:AF13)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AH13" s="41">
         <f>AG13/COUNT(C13:AF13)</f>
-        <v>1.9230769230769231</v>
+        <v>1.9285714285714286</v>
       </c>
     </row>
     <row r="14" spans="1:34">
-      <c r="A14" s="45"/>
+      <c r="A14" s="65"/>
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -5847,7 +5851,9 @@
       <c r="O14" s="1">
         <v>3</v>
       </c>
-      <c r="P14" s="1"/>
+      <c r="P14" s="1">
+        <v>7</v>
+      </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -5866,15 +5872,15 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1">
         <f>SUM(C14:AF14)</f>
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AH14" s="41">
         <f>AG14/COUNT(C14:AF14)</f>
-        <v>4</v>
+        <v>4.2142857142857144</v>
       </c>
     </row>
     <row r="15" spans="1:34">
-      <c r="A15" s="45"/>
+      <c r="A15" s="65"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -5917,7 +5923,9 @@
       <c r="O15" s="1">
         <v>2</v>
       </c>
-      <c r="P15" s="1"/>
+      <c r="P15" s="1">
+        <v>2</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -5936,11 +5944,11 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1">
         <f>SUM(C15:AF15)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AH15" s="41">
         <f>AG15/COUNT(C15:AF15)</f>
-        <v>3.2307692307692308</v>
+        <v>3.1428571428571428</v>
       </c>
     </row>
   </sheetData>
@@ -5950,89 +5958,89 @@
     <mergeCell ref="A12:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:AF7">
-    <cfRule type="top10" dxfId="59" priority="25" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="58" priority="28" operator="lessThan">
+    <cfRule type="top10" dxfId="57" priority="25" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="56" priority="28" operator="lessThan">
       <formula>$AH$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="greaterThan">
       <formula>$AH$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:AF2">
-    <cfRule type="top10" dxfId="56" priority="24" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="55" priority="26" operator="lessThan">
+    <cfRule type="top10" dxfId="54" priority="24" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="53" priority="26" operator="lessThan">
       <formula>$AH$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="greaterThan">
       <formula>$AH$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:AF9">
-    <cfRule type="top10" dxfId="53" priority="11" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="52" priority="22" operator="lessThan">
+    <cfRule type="top10" dxfId="51" priority="11" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="50" priority="22" operator="lessThan">
       <formula>$AH$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="greaterThan">
       <formula>$AH$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AF4">
-    <cfRule type="top10" dxfId="50" priority="14" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="49" priority="20" operator="lessThan">
+    <cfRule type="top10" dxfId="48" priority="14" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="47" priority="20" operator="lessThan">
       <formula>$AH$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="21" operator="greaterThan">
       <formula>$AH$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:AF5">
-    <cfRule type="top10" dxfId="47" priority="13" percent="1" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="46" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="45" priority="13" percent="1" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="44" priority="18" operator="greaterThan">
       <formula>$AH$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="lessThan">
       <formula>$AH$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:AF10">
-    <cfRule type="top10" dxfId="44" priority="12" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="43" priority="15" operator="greaterThan">
+    <cfRule type="top10" dxfId="42" priority="12" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="greaterThan">
       <formula>$AH$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="lessThan">
       <formula>$AH$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="greaterThan">
       <formula>"3,5$AG$10"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:AF12">
-    <cfRule type="top10" dxfId="40" priority="8" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="lessThan">
+    <cfRule type="top10" dxfId="38" priority="8" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
       <formula>$AH$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="greaterThan">
       <formula>$AH$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:AF14">
-    <cfRule type="top10" dxfId="37" priority="1" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThan">
+    <cfRule type="top10" dxfId="35" priority="1" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
       <formula>$AH$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
       <formula>$AH$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:AF15">
-    <cfRule type="top10" dxfId="34" priority="2" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="greaterThan">
+    <cfRule type="top10" dxfId="32" priority="2" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
       <formula>$AH$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThan">
       <formula>$AH$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="greaterThan">
       <formula>"3,5$AG$10"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6167,7 +6175,7 @@
       </c>
     </row>
     <row r="2" spans="1:38">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="65" t="s">
         <v>130</v>
       </c>
       <c r="B2" t="s">
@@ -6285,7 +6293,7 @@
       </c>
     </row>
     <row r="3" spans="1:38">
-      <c r="A3" s="45"/>
+      <c r="A3" s="65"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -6401,7 +6409,7 @@
       </c>
     </row>
     <row r="4" spans="1:38">
-      <c r="A4" s="45"/>
+      <c r="A4" s="65"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -6517,7 +6525,7 @@
       </c>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="45"/>
+      <c r="A5" s="65"/>
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -6636,7 +6644,7 @@
       <c r="AL6" s="41"/>
     </row>
     <row r="7" spans="1:38">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="65" t="s">
         <v>129</v>
       </c>
       <c r="B7" t="s">
@@ -6754,7 +6762,7 @@
       </c>
     </row>
     <row r="8" spans="1:38">
-      <c r="A8" s="45"/>
+      <c r="A8" s="65"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -6870,7 +6878,7 @@
       </c>
     </row>
     <row r="9" spans="1:38">
-      <c r="A9" s="45"/>
+      <c r="A9" s="65"/>
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -6986,7 +6994,7 @@
       </c>
     </row>
     <row r="10" spans="1:38">
-      <c r="A10" s="45"/>
+      <c r="A10" s="65"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -7105,7 +7113,7 @@
       <c r="AL11" s="41"/>
     </row>
     <row r="12" spans="1:38">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="65" t="s">
         <v>131</v>
       </c>
       <c r="B12" t="s">
@@ -7189,7 +7197,7 @@
       </c>
     </row>
     <row r="13" spans="1:38">
-      <c r="A13" s="45"/>
+      <c r="A13" s="65"/>
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -7271,7 +7279,7 @@
       </c>
     </row>
     <row r="14" spans="1:38">
-      <c r="A14" s="45"/>
+      <c r="A14" s="65"/>
       <c r="B14" t="s">
         <v>5</v>
       </c>
@@ -7353,7 +7361,7 @@
       </c>
     </row>
     <row r="15" spans="1:38">
-      <c r="A15" s="45"/>
+      <c r="A15" s="65"/>
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -7441,89 +7449,89 @@
     <mergeCell ref="A12:A15"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:AJ7">
-    <cfRule type="top10" dxfId="30" priority="25" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="lessThan">
+    <cfRule type="top10" dxfId="28" priority="25" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
       <formula>$AL$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="29" operator="greaterThan">
       <formula>$AL$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:AJ2">
-    <cfRule type="top10" dxfId="27" priority="24" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="lessThan">
+    <cfRule type="top10" dxfId="25" priority="24" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="lessThan">
       <formula>$AL$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="greaterThan">
       <formula>$AL$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:AJ9">
-    <cfRule type="top10" dxfId="24" priority="11" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="lessThan">
+    <cfRule type="top10" dxfId="22" priority="11" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
       <formula>$AL$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="greaterThan">
       <formula>$AL$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:AJ4">
-    <cfRule type="top10" dxfId="21" priority="14" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
+    <cfRule type="top10" dxfId="19" priority="14" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
       <formula>$AL$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="greaterThan">
       <formula>$AL$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:AJ5">
-    <cfRule type="top10" dxfId="18" priority="13" percent="1" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="16" priority="13" percent="1" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
       <formula>$AL$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="lessThan">
       <formula>$AL$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:AJ10">
-    <cfRule type="top10" dxfId="15" priority="12" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+    <cfRule type="top10" dxfId="13" priority="12" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>$AL$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="lessThan">
       <formula>$AL$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="greaterThan">
       <formula>"3,5$AG$10"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:AJ12">
-    <cfRule type="top10" dxfId="11" priority="8" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
+    <cfRule type="top10" dxfId="9" priority="8" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>$AL$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
       <formula>$AL$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:AJ14">
-    <cfRule type="top10" dxfId="8" priority="1" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
+    <cfRule type="top10" dxfId="6" priority="1" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
       <formula>$AL$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
       <formula>$AL$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:AJ15">
-    <cfRule type="top10" dxfId="5" priority="2" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="2" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>$AL$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
       <formula>$AL$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
       <formula>"3,5$AG$10"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new Fortuna I Liga season preparation fixes
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="421">
   <si>
     <t>bramki</t>
   </si>
@@ -1284,6 +1284,12 @@
   </si>
   <si>
     <t>2 D.Wojtyra</t>
+  </si>
+  <si>
+    <t>Cezary Sauczek</t>
+  </si>
+  <si>
+    <t>Mateusz Marzec</t>
   </si>
 </sst>
 </file>
@@ -4507,8 +4513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5578,7 +5584,9 @@
       <c r="J25" s="74" t="s">
         <v>310</v>
       </c>
-      <c r="K25" s="32"/>
+      <c r="K25" s="32" t="s">
+        <v>419</v>
+      </c>
       <c r="L25" s="74" t="s">
         <v>361</v>
       </c>
@@ -5626,7 +5634,9 @@
         <v>340</v>
       </c>
       <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
+      <c r="K26" s="74" t="s">
+        <v>420</v>
+      </c>
       <c r="L26" s="74" t="s">
         <v>362</v>
       </c>

</xml_diff>

<commit_message>
stats update, script fixes
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -4513,7 +4513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -5884,7 +5884,7 @@
   <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7261,7 +7261,9 @@
       <c r="C17" s="1">
         <v>21</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>27</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -7292,11 +7294,11 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1">
         <f>SUM(C17:AF17)</f>
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="AH17" s="41">
         <f>AG17/COUNT(C17:AF17)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
@@ -7307,7 +7309,9 @@
       <c r="C18" s="1">
         <v>5</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -7338,11 +7342,11 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1">
         <f>SUM(C18:AF18)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AH18" s="41">
         <f>AG18/COUNT(C18:AF18)</f>
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
@@ -7353,7 +7357,9 @@
       <c r="C19" s="1">
         <v>5</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -7384,11 +7390,11 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1">
         <f>SUM(C19:AF19)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AH19" s="41">
         <f>AG19/COUNT(C19:AF19)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
@@ -7399,7 +7405,9 @@
       <c r="C20" s="1">
         <v>3</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -7430,11 +7438,11 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1">
         <f>SUM(C20:AF20)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AH20" s="41">
         <f>AG20/COUNT(C20:AF20)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -7568,10 +7576,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL20"/>
+  <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7581,7 +7589,7 @@
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7691,7 +7699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7809,7 +7817,7 @@
         <v>22.529411764705884</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -7925,7 +7933,7 @@
         <v>2.6764705882352939</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8041,7 +8049,7 @@
         <v>5.3235294117647056</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8157,10 +8165,10 @@
         <v>3.6470588235294117</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AL6" s="41"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8278,7 +8286,7 @@
         <v>23.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8394,7 +8402,7 @@
         <v>2.0882352941176472</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8510,7 +8518,7 @@
         <v>4.8529411764705879</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8626,10 +8634,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AL11" s="41"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8746,8 +8754,12 @@
         <f t="shared" si="1"/>
         <v>20.970588235294116</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AN12">
+        <f>SUM(C12:AJ12)</f>
+        <v>713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -8863,7 +8875,7 @@
         <v>2.2647058823529411</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -8979,7 +8991,7 @@
         <v>6.0294117647058822</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9102,7 +9114,9 @@
       <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1">
+        <v>25</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -9138,11 +9152,11 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>0</v>
-      </c>
-      <c r="AL17" s="41" t="e">
+        <v>25</v>
+      </c>
+      <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>#DIV/0!</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
@@ -9150,7 +9164,9 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -9186,11 +9202,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>0</v>
-      </c>
-      <c r="AL18" s="41" t="e">
+        <v>4</v>
+      </c>
+      <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
@@ -9198,7 +9214,9 @@
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -9234,11 +9252,11 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>0</v>
-      </c>
-      <c r="AL19" s="41" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
@@ -9246,7 +9264,9 @@
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -9282,11 +9302,11 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>0</v>
-      </c>
-      <c r="AL20" s="41" t="e">
+        <v>2</v>
+      </c>
+      <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I liga stats update
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -7584,10 +7584,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN20"/>
+  <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7597,7 +7597,7 @@
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>22.529411764705884</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -7941,7 +7941,7 @@
         <v>2.6764705882352939</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8057,7 +8057,7 @@
         <v>5.3235294117647056</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8173,10 +8173,10 @@
         <v>3.6470588235294117</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL6" s="41"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>23.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8410,7 +8410,7 @@
         <v>2.0882352941176472</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8526,7 +8526,7 @@
         <v>4.8529411764705879</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8642,10 +8642,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL11" s="41"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8762,12 +8762,8 @@
         <f t="shared" si="1"/>
         <v>20.970588235294116</v>
       </c>
-      <c r="AN12">
-        <f>SUM(C12:AJ12)</f>
-        <v>713</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -8883,7 +8879,7 @@
         <v>2.2647058823529411</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -8999,7 +8995,7 @@
         <v>6.0294117647058822</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9128,7 +9124,9 @@
       <c r="D17" s="1">
         <v>22</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>25</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -9162,11 +9160,11 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>23.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
@@ -9180,7 +9178,9 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -9214,11 +9214,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
@@ -9232,7 +9232,9 @@
       <c r="D19" s="1">
         <v>6</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -9266,11 +9268,11 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
@@ -9284,7 +9286,9 @@
       <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -9318,11 +9322,11 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update - VI matchday
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -12,9 +17,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1290,8 +1295,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3114,44 +3119,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="H3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -3207,7 +3212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -3266,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -3325,7 +3330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="53" t="s">
         <v>23</v>
       </c>
@@ -3384,7 +3389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
         <v>24</v>
       </c>
@@ -3443,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
@@ -3502,7 +3507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -3579,7 +3584,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3598,7 +3603,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -3619,7 +3624,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3675,7 +3680,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>157</v>
@@ -3729,7 +3734,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>160</v>
@@ -3783,7 +3788,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>156</v>
@@ -3833,7 +3838,7 @@
       </c>
       <c r="S13" s="33"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>122</v>
@@ -3883,7 +3888,7 @@
       </c>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>77</v>
@@ -3927,7 +3932,7 @@
       </c>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>159</v>
@@ -3964,7 +3969,7 @@
       <c r="Q16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>158</v>
@@ -4000,7 +4005,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="37"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>110</v>
@@ -4030,7 +4035,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>145</v>
@@ -4052,7 +4057,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4071,7 +4076,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4090,7 +4095,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4108,7 +4113,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4129,7 +4134,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -4188,7 +4193,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>182</v>
@@ -4245,7 +4250,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>183</v>
@@ -4296,7 +4301,7 @@
       </c>
       <c r="S26" s="33"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>184</v>
@@ -4338,7 +4343,7 @@
       </c>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
         <v>185</v>
@@ -4372,7 +4377,7 @@
       </c>
       <c r="S28" s="33"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -4400,7 +4405,7 @@
       </c>
       <c r="S29" s="33"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4421,7 +4426,7 @@
       </c>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -4440,7 +4445,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -4459,7 +4464,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -4505,37 +4510,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -4591,7 +4596,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -4650,7 +4655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -4709,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
@@ -4768,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -4827,7 +4832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -4886,7 +4891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -4963,7 +4968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4984,7 +4989,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5005,7 +5010,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -5064,7 +5069,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>388</v>
@@ -5119,7 +5124,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>74</v>
@@ -5172,7 +5177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>259</v>
@@ -5217,7 +5222,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="36" t="s">
         <v>258</v>
@@ -5262,7 +5267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>257</v>
@@ -5299,7 +5304,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
         <v>269</v>
@@ -5330,7 +5335,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="34" t="s">
         <v>390</v>
@@ -5357,7 +5362,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5382,7 +5387,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -5404,7 +5409,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -5427,7 +5432,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -5450,7 +5455,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5470,7 +5475,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -5491,7 +5496,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -5550,7 +5555,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="74" t="s">
         <v>300</v>
@@ -5607,7 +5612,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>301</v>
@@ -5654,7 +5659,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>302</v>
@@ -5692,7 +5697,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="74" t="s">
@@ -5729,7 +5734,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="74" t="s">
@@ -5760,7 +5765,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="74" t="s">
@@ -5789,7 +5794,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -5810,7 +5815,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -5829,7 +5834,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -5875,20 +5880,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5986,7 +5991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -6092,7 +6097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6196,7 +6201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -6300,7 +6305,7 @@
         <v>4.2666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -6404,10 +6409,10 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AH6" s="42"/>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -6513,7 +6518,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6617,7 +6622,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -6721,7 +6726,7 @@
         <v>4.5333333333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -6825,10 +6830,10 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AH11" s="42"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -6934,7 +6939,7 @@
         <v>19.466666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7038,7 +7043,7 @@
         <v>2.1666666666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -7142,7 +7147,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -7246,7 +7251,7 @@
         <v>3.2666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -7265,8 +7270,12 @@
       <c r="F17" s="1">
         <v>25</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1">
+        <v>21</v>
+      </c>
+      <c r="H17" s="1">
+        <v>21</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -7293,14 +7302,14 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1">
         <f>SUM(C17:AF17)</f>
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="AH17" s="41">
         <f>AG17/COUNT(C17:AF17)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34">
+        <v>21.666666666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -7317,8 +7326,12 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -7345,14 +7358,14 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1">
         <f>SUM(C18:AF18)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="AH18" s="41">
         <f>AG18/COUNT(C18:AF18)</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -7369,8 +7382,12 @@
       <c r="F19" s="1">
         <v>5</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -7397,14 +7414,14 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1">
         <f>SUM(C19:AF19)</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="AH19" s="41">
         <f>AG19/COUNT(C19:AF19)</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34">
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -7421,8 +7438,12 @@
       <c r="F20" s="1">
         <v>4</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -7449,11 +7470,11 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1">
         <f>SUM(C20:AF20)</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="AH20" s="41">
         <f>AG20/COUNT(C20:AF20)</f>
-        <v>4</v>
+        <v>3.8333333333333335</v>
       </c>
     </row>
   </sheetData>
@@ -7586,21 +7607,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7710,7 +7731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7828,7 +7849,7 @@
         <v>22.529411764705884</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -7944,7 +7965,7 @@
         <v>2.6764705882352939</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8060,7 +8081,7 @@
         <v>5.3235294117647056</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8176,10 +8197,10 @@
         <v>3.6470588235294117</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL6" s="41"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8297,7 +8318,7 @@
         <v>23.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8413,7 +8434,7 @@
         <v>2.0882352941176472</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8529,7 +8550,7 @@
         <v>4.8529411764705879</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8645,10 +8666,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="AL11" s="41"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8766,7 +8787,7 @@
         <v>20.970588235294116</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -8882,7 +8903,7 @@
         <v>2.2647058823529411</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -8998,7 +9019,7 @@
         <v>6.0294117647058822</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9114,7 +9135,7 @@
         <v>3.8823529411764706</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -9133,8 +9154,12 @@
       <c r="F17" s="1">
         <v>14</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1">
+        <v>26</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -9165,14 +9190,14 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38">
+        <v>21.833333333333332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -9189,8 +9214,12 @@
       <c r="F18" s="1">
         <v>6</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -9221,14 +9250,14 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38">
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -9245,8 +9274,12 @@
       <c r="F19" s="1">
         <v>8</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1">
+        <v>5</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -9277,14 +9310,14 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38">
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -9301,8 +9334,12 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1">
+        <v>4</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -9333,11 +9370,11 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>2.75</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update - VII matchday part one
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -2907,7 +2907,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2942,7 +2942,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5883,7 +5883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -7611,7 +7611,7 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9160,7 +9160,9 @@
       <c r="H17" s="1">
         <v>26</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>4</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -9190,11 +9192,11 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>21.833333333333332</v>
+        <v>19.285714285714285</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
@@ -9220,7 +9222,9 @@
       <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -9250,11 +9254,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>2.1666666666666665</v>
+        <v>2.2857142857142856</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
@@ -9280,7 +9284,9 @@
       <c r="H19" s="1">
         <v>5</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>8</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -9310,11 +9316,11 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>5.333333333333333</v>
+        <v>5.7142857142857144</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
@@ -9340,7 +9346,9 @@
       <c r="H20" s="1">
         <v>4</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -9374,7 +9382,7 @@
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>3.6666666666666665</v>
+        <v>3.1428571428571428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update - VIII matchday part one
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -5884,7 +5884,7 @@
   <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7276,7 +7276,9 @@
       <c r="H17" s="1">
         <v>21</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>23</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -7302,11 +7304,11 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1">
         <f>SUM(C17:AF17)</f>
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="AH17" s="41">
         <f>AG17/COUNT(C17:AF17)</f>
-        <v>21.666666666666668</v>
+        <v>21.857142857142858</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
@@ -7332,7 +7334,9 @@
       <c r="H18" s="1">
         <v>4</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <v>6</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -7358,11 +7362,11 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1">
         <f>SUM(C18:AF18)</f>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AH18" s="41">
         <f>AG18/COUNT(C18:AF18)</f>
-        <v>2.3333333333333335</v>
+        <v>2.8571428571428572</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
@@ -7388,7 +7392,9 @@
       <c r="H19" s="1">
         <v>3</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -7414,11 +7420,11 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1">
         <f>SUM(C19:AF19)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AH19" s="41">
         <f>AG19/COUNT(C19:AF19)</f>
-        <v>4.166666666666667</v>
+        <v>4.1428571428571432</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
@@ -7444,7 +7450,9 @@
       <c r="H20" s="1">
         <v>2</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -7470,11 +7478,11 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1">
         <f>SUM(C20:AF20)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AH20" s="41">
         <f>AG20/COUNT(C20:AF20)</f>
-        <v>3.8333333333333335</v>
+        <v>3.5714285714285716</v>
       </c>
     </row>
   </sheetData>
@@ -7611,7 +7619,7 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9163,7 +9171,9 @@
       <c r="I17" s="1">
         <v>4</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>27</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -9192,11 +9202,11 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>19.285714285714285</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
@@ -9225,7 +9235,9 @@
       <c r="I18" s="1">
         <v>3</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -9254,11 +9266,11 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>2.2857142857142856</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
@@ -9287,7 +9299,9 @@
       <c r="I19" s="1">
         <v>8</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -9316,11 +9330,11 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>5.7142857142857144</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
@@ -9349,7 +9363,9 @@
       <c r="I20" s="1">
         <v>0</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -9378,11 +9394,11 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>3.1428571428571428</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update I liga
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -17,9 +12,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1295,8 +1290,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2907,7 +2902,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2942,7 +2937,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3119,44 +3114,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="H3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -3212,7 +3207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -3271,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -3330,7 +3325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="53" t="s">
         <v>23</v>
       </c>
@@ -3389,7 +3384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="57" t="s">
         <v>24</v>
       </c>
@@ -3448,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
@@ -3507,7 +3502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -3584,7 +3579,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3603,7 +3598,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -3624,7 +3619,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3680,7 +3675,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>157</v>
@@ -3734,7 +3729,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>160</v>
@@ -3788,7 +3783,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>156</v>
@@ -3838,7 +3833,7 @@
       </c>
       <c r="S13" s="33"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>122</v>
@@ -3888,7 +3883,7 @@
       </c>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>77</v>
@@ -3932,7 +3927,7 @@
       </c>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>159</v>
@@ -3969,7 +3964,7 @@
       <c r="Q16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>158</v>
@@ -4005,7 +4000,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="37"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>110</v>
@@ -4035,7 +4030,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>145</v>
@@ -4057,7 +4052,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4076,7 +4071,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4095,7 +4090,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4113,7 +4108,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4134,7 +4129,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -4193,7 +4188,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>182</v>
@@ -4250,7 +4245,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>183</v>
@@ -4301,7 +4296,7 @@
       </c>
       <c r="S26" s="33"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>184</v>
@@ -4343,7 +4338,7 @@
       </c>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
         <v>185</v>
@@ -4377,7 +4372,7 @@
       </c>
       <c r="S28" s="33"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -4405,7 +4400,7 @@
       </c>
       <c r="S29" s="33"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4426,7 +4421,7 @@
       </c>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -4445,7 +4440,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -4464,7 +4459,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -4510,37 +4505,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -4596,7 +4591,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -4655,7 +4650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -4714,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
@@ -4773,7 +4768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -4832,7 +4827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -4891,7 +4886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -4968,7 +4963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4989,7 +4984,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5010,7 +5005,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -5069,7 +5064,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>388</v>
@@ -5124,7 +5119,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>74</v>
@@ -5177,7 +5172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>259</v>
@@ -5222,7 +5217,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="36" t="s">
         <v>258</v>
@@ -5267,7 +5262,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>257</v>
@@ -5304,7 +5299,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
         <v>269</v>
@@ -5335,7 +5330,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="34" t="s">
         <v>390</v>
@@ -5362,7 +5357,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5387,7 +5382,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -5409,7 +5404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -5432,7 +5427,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -5455,7 +5450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5475,7 +5470,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -5496,7 +5491,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -5555,7 +5550,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="74" t="s">
         <v>300</v>
@@ -5612,7 +5607,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>301</v>
@@ -5659,7 +5654,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>302</v>
@@ -5697,7 +5692,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="74" t="s">
@@ -5734,7 +5729,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="74" t="s">
@@ -5765,7 +5760,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="74" t="s">
@@ -5794,7 +5789,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -5815,7 +5810,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -5834,7 +5829,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -5880,20 +5875,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5991,7 +5986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -6097,7 +6092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6201,7 +6196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -6305,7 +6300,7 @@
         <v>4.2666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -6409,10 +6404,10 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34">
       <c r="AH6" s="42"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -6518,7 +6513,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6622,7 +6617,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -6726,7 +6721,7 @@
         <v>4.5333333333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -6830,10 +6825,10 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34">
       <c r="AH11" s="42"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -6939,7 +6934,7 @@
         <v>19.466666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7043,7 +7038,7 @@
         <v>2.1666666666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -7147,7 +7142,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -7251,7 +7246,7 @@
         <v>3.2666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -7311,7 +7306,7 @@
         <v>21.857142857142858</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -7369,7 +7364,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -7427,7 +7422,7 @@
         <v>4.1428571428571432</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -7615,21 +7610,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7739,7 +7734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7857,7 +7852,7 @@
         <v>22.529411764705884</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -7973,7 +7968,7 @@
         <v>2.6764705882352939</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8089,7 +8084,7 @@
         <v>5.3235294117647056</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8205,10 +8200,10 @@
         <v>3.6470588235294117</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38">
       <c r="AL6" s="41"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8326,7 +8321,7 @@
         <v>23.823529411764707</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8442,7 +8437,7 @@
         <v>2.0882352941176472</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8558,7 +8553,7 @@
         <v>4.8529411764705879</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8674,10 +8669,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38">
       <c r="AL11" s="41"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8795,7 +8790,7 @@
         <v>20.970588235294116</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -8911,7 +8906,7 @@
         <v>2.2647058823529411</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -9027,7 +9022,7 @@
         <v>6.0294117647058822</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9143,7 +9138,7 @@
         <v>3.8823529411764706</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -9169,7 +9164,7 @@
         <v>26</v>
       </c>
       <c r="I17" s="1">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J17" s="1">
         <v>27</v>
@@ -9202,14 +9197,14 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="2">AK17/COUNT(C17:AJ17)</f>
-        <v>20.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -9233,7 +9228,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
@@ -9266,14 +9261,14 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="2"/>
-        <v>2.125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -9297,7 +9292,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J19" s="1">
         <v>4</v>
@@ -9330,14 +9325,14 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="2"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -9361,7 +9356,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1">
         <v>2</v>
@@ -9394,11 +9389,11 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>3.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update (overdue game)
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -17,9 +12,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1298,8 +1293,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2910,7 +2905,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2945,7 +2940,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3122,44 +3117,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="H3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -3333,7 +3328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="53" t="s">
         <v>23</v>
       </c>
@@ -3392,7 +3387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="57" t="s">
         <v>24</v>
       </c>
@@ -3451,7 +3446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
@@ -3510,7 +3505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -3587,7 +3582,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3606,7 +3601,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -3627,7 +3622,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3683,7 +3678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>157</v>
@@ -3737,7 +3732,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>160</v>
@@ -3791,7 +3786,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>156</v>
@@ -3841,7 +3836,7 @@
       </c>
       <c r="S13" s="33"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>122</v>
@@ -3891,7 +3886,7 @@
       </c>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>77</v>
@@ -3935,7 +3930,7 @@
       </c>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>159</v>
@@ -3972,7 +3967,7 @@
       <c r="Q16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>158</v>
@@ -4008,7 +4003,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="37"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>110</v>
@@ -4038,7 +4033,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>145</v>
@@ -4060,7 +4055,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4079,7 +4074,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4098,7 +4093,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4116,7 +4111,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4137,7 +4132,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -4196,7 +4191,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>182</v>
@@ -4253,7 +4248,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>183</v>
@@ -4304,7 +4299,7 @@
       </c>
       <c r="S26" s="33"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>184</v>
@@ -4346,7 +4341,7 @@
       </c>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
         <v>185</v>
@@ -4380,7 +4375,7 @@
       </c>
       <c r="S28" s="33"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -4408,7 +4403,7 @@
       </c>
       <c r="S29" s="33"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4429,7 +4424,7 @@
       </c>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -4448,7 +4443,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -4467,7 +4462,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -4513,37 +4508,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -4599,7 +4594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -4658,7 +4653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -4717,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
@@ -4776,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -4835,7 +4830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -4894,7 +4889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -4971,7 +4966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4992,7 +4987,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5013,7 +5008,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -5072,7 +5067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>388</v>
@@ -5127,7 +5122,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>74</v>
@@ -5180,7 +5175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>259</v>
@@ -5225,7 +5220,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="36" t="s">
         <v>258</v>
@@ -5270,7 +5265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>257</v>
@@ -5307,7 +5302,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
         <v>269</v>
@@ -5338,7 +5333,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="34" t="s">
         <v>390</v>
@@ -5365,7 +5360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5390,7 +5385,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -5412,7 +5407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -5435,7 +5430,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -5458,7 +5453,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5478,7 +5473,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -5499,7 +5494,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -5558,7 +5553,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="74" t="s">
         <v>300</v>
@@ -5615,7 +5610,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>301</v>
@@ -5662,7 +5657,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>302</v>
@@ -5700,7 +5695,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="74" t="s">
@@ -5737,7 +5732,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="74" t="s">
@@ -5768,7 +5763,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="74" t="s">
@@ -5797,7 +5792,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -5818,7 +5813,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -5837,7 +5832,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -5883,20 +5878,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK17" sqref="AK17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5997,7 +5992,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -6107,7 +6102,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6211,11 +6206,11 @@
         <v>2</v>
       </c>
       <c r="AI3" s="41">
-        <f t="shared" ref="AI3:AI20" si="1">AH3/8</f>
+        <f t="shared" ref="AI3:AI15" si="1">AH3/8</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -6323,7 +6318,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -6431,11 +6426,11 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="AH6" s="42"/>
       <c r="AI6" s="41"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -6545,7 +6540,7 @@
         <v>2.5874999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6653,7 +6648,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -6761,7 +6756,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -6869,11 +6864,11 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="AH11" s="42"/>
       <c r="AI11" s="41"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -6983,7 +6978,7 @@
         <v>2.4333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7091,7 +7086,7 @@
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -7199,7 +7194,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -7307,10 +7302,10 @@
         <v>0.40833333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="AI16" s="41"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -7327,7 +7322,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1">
         <v>21</v>
@@ -7367,18 +7362,18 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1">
         <f>SUM(C17:AF17)</f>
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="AH17" s="41">
         <f>AG17/COUNT(C17:AF17)</f>
-        <v>22.777777777777779</v>
+        <v>23.222222222222221</v>
       </c>
       <c r="AI17" s="41">
         <f>AH17/9</f>
-        <v>2.5308641975308643</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+        <v>2.5802469135802468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -7393,7 +7388,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -7433,18 +7428,18 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1">
         <f>SUM(C18:AF18)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AH18" s="41">
         <f>AG18/COUNT(C18:AF18)</f>
-        <v>2.4444444444444446</v>
+        <v>2.5555555555555554</v>
       </c>
       <c r="AI18" s="41">
         <f>AH18/9</f>
-        <v>0.27160493827160498</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+        <v>0.2839506172839506</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -7510,7 +7505,7 @@
         <v>0.48148148148148145</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -7706,21 +7701,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7833,7 +7828,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7955,7 +7950,7 @@
         <v>2.5032679738562091</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -8075,7 +8070,7 @@
         <v>0.33455882352941174</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8195,7 +8190,7 @@
         <v>0.6654411764705882</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8315,11 +8310,11 @@
         <v>0.45588235294117646</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39">
       <c r="AL6" s="41"/>
       <c r="AM6" s="41"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8441,7 +8436,7 @@
         <v>2.9779411764705883</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8561,7 +8556,7 @@
         <v>0.2610294117647059</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8681,7 +8676,7 @@
         <v>0.60661764705882348</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8801,11 +8796,11 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39">
       <c r="AL11" s="41"/>
       <c r="AM11" s="41"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8927,7 +8922,7 @@
         <v>2.6213235294117645</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -9047,7 +9042,7 @@
         <v>0.28308823529411764</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -9167,7 +9162,7 @@
         <v>0.75367647058823528</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9287,10 +9282,10 @@
         <v>0.48529411764705882</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39">
       <c r="AM16" s="41"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -9364,7 +9359,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -9436,7 +9431,7 @@
         <v>0.28749999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -9508,7 +9503,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
stats update, merge fixes
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -12,9 +17,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1293,8 +1298,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3117,44 +3122,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="H3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.36328125" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -3328,7 +3333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="53" t="s">
         <v>23</v>
       </c>
@@ -3387,7 +3392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
         <v>24</v>
       </c>
@@ -3446,7 +3451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
@@ -3505,7 +3510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -3582,7 +3587,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3601,7 +3606,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -3622,7 +3627,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3678,7 +3683,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>157</v>
@@ -3732,7 +3737,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>160</v>
@@ -3786,7 +3791,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>156</v>
@@ -3836,7 +3841,7 @@
       </c>
       <c r="S13" s="33"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>122</v>
@@ -3886,7 +3891,7 @@
       </c>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>77</v>
@@ -3930,7 +3935,7 @@
       </c>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>159</v>
@@ -3967,7 +3972,7 @@
       <c r="Q16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>158</v>
@@ -4003,7 +4008,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="37"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>110</v>
@@ -4033,7 +4038,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>145</v>
@@ -4055,7 +4060,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4074,7 +4079,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4093,7 +4098,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4111,7 +4116,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4132,7 +4137,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -4191,7 +4196,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>182</v>
@@ -4248,7 +4253,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>183</v>
@@ -4299,7 +4304,7 @@
       </c>
       <c r="S26" s="33"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>184</v>
@@ -4341,7 +4346,7 @@
       </c>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
         <v>185</v>
@@ -4375,7 +4380,7 @@
       </c>
       <c r="S28" s="33"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -4403,7 +4408,7 @@
       </c>
       <c r="S29" s="33"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4424,7 +4429,7 @@
       </c>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -4443,7 +4448,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -4462,7 +4467,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -4508,37 +4513,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -4594,7 +4599,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -4653,7 +4658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -4712,7 +4717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
@@ -4771,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1">
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -4830,7 +4835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -4889,7 +4894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -4966,7 +4971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4987,7 +4992,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5008,7 +5013,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -5067,7 +5072,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>388</v>
@@ -5122,7 +5127,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>74</v>
@@ -5175,7 +5180,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>259</v>
@@ -5220,7 +5225,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="31"/>
       <c r="B14" s="36" t="s">
         <v>258</v>
@@ -5265,7 +5270,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>257</v>
@@ -5302,7 +5307,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
         <v>269</v>
@@ -5333,7 +5338,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="31"/>
       <c r="B17" s="34" t="s">
         <v>390</v>
@@ -5360,7 +5365,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5385,7 +5390,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -5407,7 +5412,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -5430,7 +5435,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -5453,7 +5458,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5473,7 +5478,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -5494,7 +5499,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -5553,7 +5558,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="74" t="s">
         <v>300</v>
@@ -5610,7 +5615,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>301</v>
@@ -5657,7 +5662,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>302</v>
@@ -5695,7 +5700,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="74" t="s">
@@ -5732,7 +5737,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="74" t="s">
@@ -5763,7 +5768,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="74" t="s">
@@ -5792,7 +5797,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -5813,7 +5818,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -5832,7 +5837,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1">
+    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -5878,20 +5883,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5992,7 +5997,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -6102,7 +6107,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6210,7 +6215,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -6318,7 +6323,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -6426,11 +6431,11 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AH6" s="42"/>
       <c r="AI6" s="41"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -6540,7 +6545,7 @@
         <v>2.5874999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6648,7 +6653,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -6756,7 +6761,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -6864,11 +6869,11 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AH11" s="42"/>
       <c r="AI11" s="41"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -6978,7 +6983,7 @@
         <v>2.4333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7086,7 +7091,7 @@
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -7194,7 +7199,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -7302,10 +7307,10 @@
         <v>0.40833333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AI16" s="41"/>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -7339,7 +7344,9 @@
       <c r="K17" s="1">
         <v>28</v>
       </c>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1">
+        <v>32</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -7362,18 +7369,18 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1">
         <f>SUM(C17:AF17)</f>
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="AH17" s="41">
         <f>AG17/COUNT(C17:AF17)</f>
-        <v>23.222222222222221</v>
+        <v>24.1</v>
       </c>
       <c r="AI17" s="41">
         <f>AH17/9</f>
-        <v>2.5802469135802468</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35">
+        <v>2.677777777777778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -7405,7 +7412,9 @@
       <c r="K18" s="1">
         <v>0</v>
       </c>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -7428,18 +7437,18 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1">
         <f>SUM(C18:AF18)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AH18" s="41">
         <f>AG18/COUNT(C18:AF18)</f>
-        <v>2.5555555555555554</v>
+        <v>2.5</v>
       </c>
       <c r="AI18" s="41">
         <f>AH18/9</f>
-        <v>0.2839506172839506</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35">
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -7471,7 +7480,9 @@
       <c r="K19" s="1">
         <v>5</v>
       </c>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <v>4</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -7494,18 +7505,18 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1">
         <f>SUM(C19:AF19)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AH19" s="41">
         <f>AG19/COUNT(C19:AF19)</f>
-        <v>4.333333333333333</v>
+        <v>4.3</v>
       </c>
       <c r="AI19" s="41">
         <f>AH19/9</f>
-        <v>0.48148148148148145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35">
+        <v>0.47777777777777775</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -7537,7 +7548,9 @@
       <c r="K20" s="1">
         <v>4</v>
       </c>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1">
+        <v>6</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -7560,15 +7573,15 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1">
         <f>SUM(C20:AF20)</f>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AH20" s="41">
         <f>AG20/COUNT(C20:AF20)</f>
-        <v>3.8888888888888888</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AI20" s="41">
         <f>AH20/9</f>
-        <v>0.43209876543209874</v>
+        <v>0.45555555555555549</v>
       </c>
     </row>
   </sheetData>
@@ -7701,21 +7714,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AM2" sqref="AM2"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7828,7 +7841,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7950,7 +7963,7 @@
         <v>2.5032679738562091</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -8070,7 +8083,7 @@
         <v>0.33455882352941174</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8190,7 +8203,7 @@
         <v>0.6654411764705882</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8310,11 +8323,11 @@
         <v>0.45588235294117646</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="AL6" s="41"/>
       <c r="AM6" s="41"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8436,7 +8449,7 @@
         <v>2.9779411764705883</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8556,7 +8569,7 @@
         <v>0.2610294117647059</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8676,7 +8689,7 @@
         <v>0.60661764705882348</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8796,11 +8809,11 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="AL11" s="41"/>
       <c r="AM11" s="41"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8922,7 +8935,7 @@
         <v>2.6213235294117645</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -9042,7 +9055,7 @@
         <v>0.28308823529411764</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -9162,7 +9175,7 @@
         <v>0.75367647058823528</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9282,10 +9295,10 @@
         <v>0.48529411764705882</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="AM16" s="41"/>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -9322,7 +9335,9 @@
       <c r="L17" s="1">
         <v>21</v>
       </c>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>25</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -9348,18 +9363,18 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="3">AK17/COUNT(C17:AJ17)</f>
-        <v>21.6</v>
+        <v>21.90909090909091</v>
       </c>
       <c r="AM17" s="41">
         <f t="shared" si="1"/>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39">
+        <v>2.7386363636363638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -9394,7 +9409,9 @@
       <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="M18" s="1"/>
+      <c r="M18" s="1">
+        <v>2</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -9420,18 +9437,18 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="3"/>
-        <v>2.2999999999999998</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="AM18" s="41">
         <f t="shared" si="1"/>
-        <v>0.28749999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:39">
+        <v>0.28409090909090912</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -9466,7 +9483,9 @@
       <c r="L19" s="1">
         <v>9</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1">
+        <v>5</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -9492,18 +9511,18 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="3"/>
-        <v>5.6</v>
+        <v>5.5454545454545459</v>
       </c>
       <c r="AM19" s="41">
         <f t="shared" si="1"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:39">
+        <v>0.69318181818181823</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -9538,7 +9557,9 @@
       <c r="L20" s="1">
         <v>6</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1">
+        <v>3</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -9564,15 +9585,15 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="3"/>
-        <v>3.3</v>
+        <v>3.2727272727272729</v>
       </c>
       <c r="AM20" s="41">
         <f t="shared" si="1"/>
-        <v>0.41249999999999998</v>
+        <v>0.40909090909090912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update, weighted stats improvement
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -2910,7 +2910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2945,7 +2945,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5886,7 +5886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -7717,8 +7717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9338,7 +9338,9 @@
       <c r="M17" s="1">
         <v>25</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>13</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -9363,15 +9365,15 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="3">AK17/COUNT(C17:AJ17)</f>
-        <v>21.90909090909091</v>
+        <v>21.166666666666668</v>
       </c>
       <c r="AM17" s="41">
         <f t="shared" si="1"/>
-        <v>2.7386363636363638</v>
+        <v>2.6458333333333335</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
@@ -9412,7 +9414,9 @@
       <c r="M18" s="1">
         <v>2</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>2</v>
+      </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -9437,15 +9441,15 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="3"/>
-        <v>2.2727272727272729</v>
+        <v>2.25</v>
       </c>
       <c r="AM18" s="41">
         <f t="shared" si="1"/>
-        <v>0.28409090909090912</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
@@ -9486,7 +9490,9 @@
       <c r="M19" s="1">
         <v>5</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>3</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -9511,15 +9517,15 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="3"/>
-        <v>5.5454545454545459</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="AM19" s="41">
         <f t="shared" si="1"/>
-        <v>0.69318181818181823</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
@@ -9560,7 +9566,9 @@
       <c r="M20" s="1">
         <v>3</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -9585,15 +9593,15 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="3"/>
-        <v>3.2727272727272729</v>
+        <v>3.0833333333333335</v>
       </c>
       <c r="AM20" s="41">
         <f t="shared" si="1"/>
-        <v>0.40909090909090912</v>
+        <v>0.38541666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stats update (overdue games)
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\EkstraModel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -17,9 +12,9 @@
     <sheet name="Sezony Ekstra" sheetId="1" r:id="rId3"/>
     <sheet name="Sezony I liga" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1298,8 +1293,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2910,7 +2905,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2945,7 +2940,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3122,44 +3117,44 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="H3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:S33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -3215,7 +3210,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -3274,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
@@ -3333,7 +3328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="53" t="s">
         <v>23</v>
       </c>
@@ -3392,7 +3387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="57" t="s">
         <v>24</v>
       </c>
@@ -3451,7 +3446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="61" t="s">
         <v>25</v>
       </c>
@@ -3510,7 +3505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -3587,7 +3582,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3606,7 +3601,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -3627,7 +3622,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -3683,7 +3678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>157</v>
@@ -3737,7 +3732,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>160</v>
@@ -3791,7 +3786,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>156</v>
@@ -3841,7 +3836,7 @@
       </c>
       <c r="S13" s="33"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="32" t="s">
         <v>122</v>
@@ -3891,7 +3886,7 @@
       </c>
       <c r="S14" s="33"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>77</v>
@@ -3935,7 +3930,7 @@
       </c>
       <c r="S15" s="33"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="34" t="s">
         <v>159</v>
@@ -3972,7 +3967,7 @@
       <c r="Q16" s="32"/>
       <c r="S16" s="33"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="32" t="s">
         <v>158</v>
@@ -4008,7 +4003,7 @@
       <c r="R17" s="32"/>
       <c r="S17" s="37"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
         <v>110</v>
@@ -4038,7 +4033,7 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34" t="s">
         <v>145</v>
@@ -4060,7 +4055,7 @@
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -4079,7 +4074,7 @@
       <c r="R20" s="36"/>
       <c r="S20" s="37"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -4098,7 +4093,7 @@
       <c r="R21" s="36"/>
       <c r="S21" s="37"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -4116,7 +4111,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -4137,7 +4132,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -4196,7 +4191,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="32" t="s">
         <v>182</v>
@@ -4253,7 +4248,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>183</v>
@@ -4304,7 +4299,7 @@
       </c>
       <c r="S26" s="33"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>184</v>
@@ -4346,7 +4341,7 @@
       </c>
       <c r="S27" s="33"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32" t="s">
         <v>185</v>
@@ -4380,7 +4375,7 @@
       </c>
       <c r="S28" s="33"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -4408,7 +4403,7 @@
       </c>
       <c r="S29" s="33"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4429,7 +4424,7 @@
       </c>
       <c r="S30" s="33"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -4448,7 +4443,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -4467,7 +4462,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -4513,37 +4508,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>36</v>
       </c>
@@ -4599,7 +4594,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -4658,7 +4653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" ht="15" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
@@ -4717,7 +4712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
@@ -4776,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="15" thickBot="1">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -4835,7 +4830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="15" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
@@ -4894,7 +4889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15" thickBot="1">
       <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
@@ -4971,7 +4966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -4992,7 +4987,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="24"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="15" thickBot="1">
       <c r="A9" s="25"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
@@ -5013,7 +5008,7 @@
       <c r="R9" s="26"/>
       <c r="S9" s="27"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19">
       <c r="A10" s="28" t="s">
         <v>27</v>
       </c>
@@ -5072,7 +5067,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19">
       <c r="A11" s="31"/>
       <c r="B11" s="32" t="s">
         <v>388</v>
@@ -5127,7 +5122,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="A12" s="31"/>
       <c r="B12" s="32" t="s">
         <v>74</v>
@@ -5180,7 +5175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="A13" s="35"/>
       <c r="B13" s="32" t="s">
         <v>259</v>
@@ -5225,7 +5220,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="A14" s="31"/>
       <c r="B14" s="36" t="s">
         <v>258</v>
@@ -5270,7 +5265,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19">
       <c r="A15" s="31"/>
       <c r="B15" s="32" t="s">
         <v>257</v>
@@ -5307,7 +5302,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
         <v>269</v>
@@ -5338,7 +5333,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19">
       <c r="A17" s="31"/>
       <c r="B17" s="34" t="s">
         <v>390</v>
@@ -5365,7 +5360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19">
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5390,7 +5385,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19">
       <c r="A19" s="35"/>
       <c r="B19" s="34"/>
       <c r="C19" s="36"/>
@@ -5412,7 +5407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19">
       <c r="A20" s="35"/>
       <c r="B20" s="32"/>
       <c r="C20" s="36"/>
@@ -5435,7 +5430,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19">
       <c r="A21" s="35"/>
       <c r="B21" s="36"/>
       <c r="C21" s="36"/>
@@ -5458,7 +5453,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19">
       <c r="A22" s="35"/>
       <c r="B22" s="36"/>
       <c r="C22" s="36"/>
@@ -5478,7 +5473,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="37"/>
     </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="15" thickBot="1">
       <c r="A23" s="25"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
@@ -5499,7 +5494,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="39"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19">
       <c r="A24" s="28" t="s">
         <v>28</v>
       </c>
@@ -5558,7 +5553,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19">
       <c r="A25" s="35"/>
       <c r="B25" s="74" t="s">
         <v>300</v>
@@ -5615,7 +5610,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19">
       <c r="A26" s="35"/>
       <c r="B26" s="32" t="s">
         <v>301</v>
@@ -5662,7 +5657,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19">
       <c r="A27" s="31"/>
       <c r="B27" s="32" t="s">
         <v>302</v>
@@ -5700,7 +5695,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
       <c r="C28" s="74" t="s">
@@ -5737,7 +5732,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19">
       <c r="A29" s="31"/>
       <c r="B29" s="32"/>
       <c r="C29" s="74" t="s">
@@ -5768,7 +5763,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="74" t="s">
@@ -5797,7 +5792,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19">
       <c r="A31" s="31"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -5818,7 +5813,7 @@
       <c r="R31" s="32"/>
       <c r="S31" s="33"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
@@ -5837,7 +5832,7 @@
       <c r="R32" s="32"/>
       <c r="S32" s="33"/>
     </row>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" ht="15" thickBot="1">
       <c r="A33" s="40"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -5883,20 +5878,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -5997,7 +5992,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -6107,7 +6102,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -6215,7 +6210,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -6323,7 +6318,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -6431,11 +6426,11 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35">
       <c r="AH6" s="42"/>
       <c r="AI6" s="41"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -6545,7 +6540,7 @@
         <v>2.5874999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -6653,7 +6648,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -6761,7 +6756,7 @@
         <v>0.56666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -6869,11 +6864,11 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35">
       <c r="AH11" s="42"/>
       <c r="AI11" s="41"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -6983,7 +6978,7 @@
         <v>2.4333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -7091,7 +7086,7 @@
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -7199,7 +7194,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -7307,10 +7302,10 @@
         <v>0.40833333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35">
       <c r="AI16" s="41"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -7382,7 +7377,7 @@
         <v>2.6363636363636362</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -7452,7 +7447,7 @@
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -7522,7 +7517,7 @@
         <v>0.48484848484848481</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -7722,21 +7717,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="32" width="3" bestFit="1" customWidth="1"/>
     <col min="33" max="36" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39">
       <c r="C1" s="2">
         <v>1</v>
       </c>
@@ -7849,7 +7844,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39">
       <c r="A2" s="79" t="s">
         <v>54</v>
       </c>
@@ -7971,7 +7966,7 @@
         <v>2.5032679738562091</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39">
       <c r="A3" s="79"/>
       <c r="B3" t="s">
         <v>1</v>
@@ -8091,7 +8086,7 @@
         <v>0.33455882352941174</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39">
       <c r="A4" s="79"/>
       <c r="B4" t="s">
         <v>4</v>
@@ -8211,7 +8206,7 @@
         <v>0.6654411764705882</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39">
       <c r="A5" s="79"/>
       <c r="B5" t="s">
         <v>20</v>
@@ -8331,11 +8326,11 @@
         <v>0.45588235294117646</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39">
       <c r="AL6" s="41"/>
       <c r="AM6" s="41"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39">
       <c r="A7" s="79" t="s">
         <v>53</v>
       </c>
@@ -8457,7 +8452,7 @@
         <v>2.9779411764705883</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39">
       <c r="A8" s="79"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -8577,7 +8572,7 @@
         <v>0.2610294117647059</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39">
       <c r="A9" s="79"/>
       <c r="B9" t="s">
         <v>4</v>
@@ -8697,7 +8692,7 @@
         <v>0.60661764705882348</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39">
       <c r="A10" s="79"/>
       <c r="B10" t="s">
         <v>20</v>
@@ -8817,11 +8812,11 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39">
       <c r="AL11" s="41"/>
       <c r="AM11" s="41"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39">
       <c r="A12" s="79" t="s">
         <v>55</v>
       </c>
@@ -8943,7 +8938,7 @@
         <v>2.6213235294117645</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39">
       <c r="A13" s="79"/>
       <c r="B13" t="s">
         <v>1</v>
@@ -9063,7 +9058,7 @@
         <v>0.28308823529411764</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39">
       <c r="A14" s="79"/>
       <c r="B14" t="s">
         <v>4</v>
@@ -9183,7 +9178,7 @@
         <v>0.75367647058823528</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39">
       <c r="A15" s="79"/>
       <c r="B15" t="s">
         <v>20</v>
@@ -9303,10 +9298,10 @@
         <v>0.48529411764705882</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39">
       <c r="AM16" s="41"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39">
       <c r="A17" s="79" t="s">
         <v>249</v>
       </c>
@@ -9347,7 +9342,7 @@
         <v>25</v>
       </c>
       <c r="N17" s="1">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="O17" s="1">
         <v>20</v>
@@ -9375,18 +9370,18 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="3">AK17/COUNT(C17:AJ17)</f>
-        <v>21.076923076923077</v>
+        <v>21.692307692307693</v>
       </c>
       <c r="AM17" s="41">
         <f t="shared" si="1"/>
-        <v>2.6346153846153846</v>
-      </c>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
+        <v>2.7115384615384617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39">
       <c r="A18" s="79"/>
       <c r="B18" t="s">
         <v>1</v>
@@ -9464,7 +9459,7 @@
         <v>0.26923076923076922</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39">
       <c r="A19" s="79"/>
       <c r="B19" t="s">
         <v>4</v>
@@ -9503,7 +9498,7 @@
         <v>5</v>
       </c>
       <c r="N19" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O19" s="1">
         <v>8</v>
@@ -9531,18 +9526,18 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="3"/>
-        <v>5.5384615384615383</v>
+        <v>5.6923076923076925</v>
       </c>
       <c r="AM19" s="41">
         <f t="shared" si="1"/>
-        <v>0.69230769230769229</v>
-      </c>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
+        <v>0.71153846153846156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39">
       <c r="A20" s="79"/>
       <c r="B20" t="s">
         <v>20</v>
@@ -9581,7 +9576,7 @@
         <v>3</v>
       </c>
       <c r="N20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O20" s="1">
         <v>5</v>
@@ -9609,15 +9604,15 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="3"/>
-        <v>3.2307692307692308</v>
+        <v>3.3076923076923075</v>
       </c>
       <c r="AM20" s="41">
         <f t="shared" si="1"/>
-        <v>0.40384615384615385</v>
+        <v>0.41346153846153844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I liga spring round preparation
</commit_message>
<xml_diff>
--- a/Vademecum.xlsx
+++ b/Vademecum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sparingi Ekstra" sheetId="2" r:id="rId1"/>
@@ -5886,8 +5886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7805,8 +7805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9450,7 +9450,9 @@
       <c r="U17" s="1">
         <v>23</v>
       </c>
-      <c r="V17" s="44"/>
+      <c r="V17" s="44">
+        <v>22</v>
+      </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -9467,15 +9469,15 @@
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f>SUM(C17:AJ17)</f>
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="AL17" s="41">
         <f t="shared" ref="AL17:AL20" si="3">AK17/COUNT(C17:AJ17)</f>
-        <v>22.105263157894736</v>
+        <v>22.1</v>
       </c>
       <c r="AM17" s="41">
         <f t="shared" si="1"/>
-        <v>2.763157894736842</v>
+        <v>2.7625000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
@@ -9540,7 +9542,9 @@
       <c r="U18" s="1">
         <v>3</v>
       </c>
-      <c r="V18" s="44"/>
+      <c r="V18" s="44">
+        <v>1</v>
+      </c>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -9557,15 +9561,15 @@
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f>SUM(C18:AJ18)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL18" s="41">
         <f t="shared" si="3"/>
-        <v>2.4736842105263159</v>
+        <v>2.4</v>
       </c>
       <c r="AM18" s="41">
         <f t="shared" si="1"/>
-        <v>0.30921052631578949</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.3">
@@ -9630,7 +9634,9 @@
       <c r="U19" s="1">
         <v>4</v>
       </c>
-      <c r="V19" s="44"/>
+      <c r="V19" s="44">
+        <v>7</v>
+      </c>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -9647,15 +9653,15 @@
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f>SUM(C19:AJ19)</f>
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="AL19" s="41">
         <f t="shared" si="3"/>
-        <v>5.7894736842105265</v>
+        <v>5.85</v>
       </c>
       <c r="AM19" s="41">
         <f t="shared" si="1"/>
-        <v>0.72368421052631582</v>
+        <v>0.73124999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
@@ -9720,7 +9726,9 @@
       <c r="U20" s="1">
         <v>3</v>
       </c>
-      <c r="V20" s="44"/>
+      <c r="V20" s="44">
+        <v>3</v>
+      </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -9737,15 +9745,15 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f>SUM(C20:AJ20)</f>
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AL20" s="41">
         <f t="shared" si="3"/>
-        <v>3.6315789473684212</v>
+        <v>3.6</v>
       </c>
       <c r="AM20" s="41">
         <f t="shared" si="1"/>
-        <v>0.45394736842105265</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>